<commit_message>
Crear cuentas de est por exel, inscribirlos, controlar que no se inscriban a la misma 2 veces, controlar que se inscriban area, cat y grado ed la convocatoria y mostrar un resumend e toda la convocatoria mas descargar plantilla arreglado v2
</commit_message>
<xml_diff>
--- a/public/plantillasExel/plantilla_inscripcion.xlsx
+++ b/public/plantillasExel/plantilla_inscripcion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E36F61F-7DC5-475C-B56E-D415CD005300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F77E42E-BA11-4922-85BB-4BD2B5E7B7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla Estudiantes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Nombre</t>
   </si>
@@ -67,9 +67,6 @@
     <t>ApellidoM1</t>
   </si>
   <si>
-    <t>CI123456</t>
-  </si>
-  <si>
     <t>ejemplo1@email.com</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>ApellidoM2</t>
   </si>
   <si>
-    <t>CI654321</t>
-  </si>
-  <si>
     <t>ejemplo2@email.com</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
   </si>
   <si>
     <t>ApellidoM3</t>
-  </si>
-  <si>
-    <t>CI789012</t>
   </si>
   <si>
     <t>ejemplo3@email.com</t>
@@ -512,7 +503,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,108 +566,108 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>123456</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="F2" s="1">
         <v>38579</v>
       </c>
       <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3">
+        <v>654321</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="F3" s="1">
         <v>38847</v>
       </c>
       <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4">
+        <v>789012</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="F4" s="1">
         <v>39161</v>
       </c>
       <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correciones en registrar lista de excel
</commit_message>
<xml_diff>
--- a/public/plantillasExel/plantilla_inscripcion.xlsx
+++ b/public/plantillasExel/plantilla_inscripcion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F77E42E-BA11-4922-85BB-4BD2B5E7B7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73752A69-5689-4B44-A452-47F6F34D54B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla Estudiantes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>Nombre</t>
   </si>
@@ -58,95 +58,134 @@
     <t>Delegación</t>
   </si>
   <si>
-    <t>EjemploNombre1</t>
-  </si>
-  <si>
-    <t>ApellidoP1</t>
-  </si>
-  <si>
-    <t>ApellidoM1</t>
-  </si>
-  <si>
-    <t>ejemplo1@email.com</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>ÁreaEjemplo1</t>
-  </si>
-  <si>
-    <t>70000001</t>
-  </si>
-  <si>
-    <t>DelegaciónEjemplo1</t>
-  </si>
-  <si>
-    <t>EjemploNombre2</t>
-  </si>
-  <si>
-    <t>ApellidoP2</t>
-  </si>
-  <si>
-    <t>ApellidoM2</t>
-  </si>
-  <si>
-    <t>ejemplo2@email.com</t>
+    <t>Unidad Educativa San Martín</t>
+  </si>
+  <si>
+    <t>1ro de Secundaria</t>
+  </si>
+  <si>
+    <t>2002-03-04</t>
+  </si>
+  <si>
+    <t>2002-03-05</t>
+  </si>
+  <si>
+    <t>2002-03-06</t>
+  </si>
+  <si>
+    <t>2002/03/03</t>
+  </si>
+  <si>
+    <t>Nombre y Apellidos del tutor</t>
+  </si>
+  <si>
+    <t>Correo del tutor</t>
+  </si>
+  <si>
+    <t>tutorPadreENCARAGDO@GMAIL</t>
+  </si>
+  <si>
+    <t>Estudiante1</t>
+  </si>
+  <si>
+    <t>Estudiante2</t>
+  </si>
+  <si>
+    <t>Estudiante3</t>
+  </si>
+  <si>
+    <t>Estudiante4</t>
+  </si>
+  <si>
+    <t>ApellidoPaterno1</t>
+  </si>
+  <si>
+    <t>ApellidoPaterno2</t>
+  </si>
+  <si>
+    <t>ApellidoPaterno3</t>
+  </si>
+  <si>
+    <t>ApellidoPaterno4</t>
+  </si>
+  <si>
+    <t>ApellidoMaterno1</t>
+  </si>
+  <si>
+    <t>ApellidoMaterno2</t>
+  </si>
+  <si>
+    <t>ApellidoMaterno3</t>
+  </si>
+  <si>
+    <t>ApellidoMaterno4</t>
+  </si>
+  <si>
+    <t>correo1@gmail.com</t>
+  </si>
+  <si>
+    <t>correo2@gmail.com</t>
+  </si>
+  <si>
+    <t>correo3@gmail.com</t>
+  </si>
+  <si>
+    <t>correo4@gmail.com</t>
   </si>
   <si>
     <t>F</t>
   </si>
   <si>
-    <t>ÁreaEjemplo2</t>
-  </si>
-  <si>
-    <t>70000002</t>
-  </si>
-  <si>
-    <t>DelegaciónEjemplo2</t>
-  </si>
-  <si>
-    <t>EjemploNombre3</t>
-  </si>
-  <si>
-    <t>ApellidoP3</t>
-  </si>
-  <si>
-    <t>ApellidoM3</t>
-  </si>
-  <si>
-    <t>ejemplo3@email.com</t>
-  </si>
-  <si>
-    <t>70000003</t>
-  </si>
-  <si>
-    <t>1p</t>
+    <t>Área1</t>
+  </si>
+  <si>
+    <t>Área2</t>
+  </si>
+  <si>
+    <t>Área3</t>
+  </si>
+  <si>
+    <t>Área4</t>
+  </si>
+  <si>
+    <t>Categoria1</t>
+  </si>
+  <si>
+    <t>Categoria2</t>
+  </si>
+  <si>
+    <t>Categoria3</t>
+  </si>
+  <si>
+    <t>Categoria4</t>
+  </si>
+  <si>
+    <t>2do de Primaria</t>
   </si>
   <si>
     <t>3ro de Primaria</t>
   </si>
   <si>
-    <t>1ro de Primaria</t>
-  </si>
-  <si>
-    <t>2do de Primaria</t>
-  </si>
-  <si>
-    <t>2p</t>
-  </si>
-  <si>
-    <t>3p</t>
+    <t>Nombre Apellidos tutor1</t>
+  </si>
+  <si>
+    <t>Nombre Apellidos tutor2</t>
+  </si>
+  <si>
+    <t>Nombre Apellidos tutor3</t>
+  </si>
+  <si>
+    <t>Nombre Apellidos tutor4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +205,19 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -192,11 +244,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -500,182 +554,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
     <col min="8" max="8" width="12.140625" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" customWidth="1"/>
+    <col min="12" max="12" width="29" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" customWidth="1"/>
+    <col min="14" max="14" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>12345679</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2">
+        <v>63887464</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>12345679</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3">
+        <v>63887464</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>12345679</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4">
+        <v>63887464</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="M4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>12345679</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" t="s">
         <v>14</v>
       </c>
-      <c r="D2">
-        <v>123456</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1">
-        <v>38579</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="K5">
+        <v>63887464</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3">
-        <v>654321</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="1">
-        <v>38847</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>789012</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="1">
-        <v>39161</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{95442933-8AE4-41E2-91B4-DA52240AC78B}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{BC04D35A-A242-4B82-A7E8-31B13D4445FC}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{EBF7CD42-7FB8-4CAD-B025-E2F92AB7DFBB}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{3B374B01-F81A-45AC-AFAA-0B896D3AEA88}"/>
+    <hyperlink ref="N2" r:id="rId2" xr:uid="{9B4B4810-6E59-49C0-8AE5-A1E2860537F5}"/>
+    <hyperlink ref="N3" r:id="rId3" xr:uid="{83196340-12AD-4EB7-A211-12A7E0958961}"/>
+    <hyperlink ref="N4" r:id="rId4" xr:uid="{B17A8E36-C399-4E49-B0DC-C793DBCEA39D}"/>
+    <hyperlink ref="N5" r:id="rId5" xr:uid="{BFFE8C52-F7CA-4440-B140-C9498842ED6C}"/>
+    <hyperlink ref="E3:E5" r:id="rId6" display="t9@gmail.com" xr:uid="{00100EBB-8124-4249-8F82-0CDCC3E476E8}"/>
+    <hyperlink ref="E3" r:id="rId7" xr:uid="{5F59B778-E74F-434D-9676-0F736C1303A2}"/>
+    <hyperlink ref="E4" r:id="rId8" xr:uid="{38C3091A-71F6-4B27-BD5A-DF91006D84BA}"/>
+    <hyperlink ref="E5" r:id="rId9" xr:uid="{45EC7D2B-9946-4C55-A87D-98AB6A48BD5F}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>